<commit_message>
idk just fixed some stuff
</commit_message>
<xml_diff>
--- a/downloads/file.xlsx
+++ b/downloads/file.xlsx
@@ -1,17 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1000001_{F0D7379A-EBFF-404A-ABB2-5B16759B41C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="0" yWindow="0" windowWidth="0" windowHeight="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="191028"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="43">
   <si>
     <t xml:space="preserve">الاسم </t>
   </si>
@@ -134,20 +151,27 @@
   </si>
   <si>
     <t>تجديد ممارسه مع عيادة</t>
+  </si>
+  <si>
+    <t>محمد تحسين طاهر</t>
+  </si>
+  <si>
+    <t>مدري وش يعني معامله</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
@@ -158,7 +182,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -168,35 +192,40 @@
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -386,23 +415,28 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:B34"/>
   <sheetViews>
-    <sheetView rightToLeft="1" workbookViewId="0"/>
+    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="B34" sqref="B34"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="12.67578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col customWidth="1" min="1" max="2" width="18.25"/>
+    <col min="1" max="2" width="18.203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -410,7 +444,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:2" ht="12.75" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -418,7 +452,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:2" ht="12.75" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
@@ -426,7 +460,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:2" ht="12.75" x14ac:dyDescent="0.15">
       <c r="A4" s="2" t="s">
         <v>5</v>
       </c>
@@ -434,7 +468,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:2" ht="12.75" x14ac:dyDescent="0.15">
       <c r="A5" s="2" t="s">
         <v>6</v>
       </c>
@@ -442,7 +476,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:2" ht="12.75" x14ac:dyDescent="0.15">
       <c r="A6" s="2" t="s">
         <v>7</v>
       </c>
@@ -450,7 +484,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:2" ht="12.75" x14ac:dyDescent="0.15">
       <c r="A7" s="2" t="s">
         <v>8</v>
       </c>
@@ -458,7 +492,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:2" ht="12.75" x14ac:dyDescent="0.15">
       <c r="A8" s="2" t="s">
         <v>9</v>
       </c>
@@ -466,7 +500,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:2" ht="12.75" x14ac:dyDescent="0.15">
       <c r="A9" s="2" t="s">
         <v>10</v>
       </c>
@@ -474,7 +508,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:2" ht="12.75" x14ac:dyDescent="0.15">
       <c r="A10" s="2" t="s">
         <v>11</v>
       </c>
@@ -482,7 +516,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" spans="1:2" ht="12.75" x14ac:dyDescent="0.15">
       <c r="A11" s="2" t="s">
         <v>13</v>
       </c>
@@ -490,7 +524,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" spans="1:2" ht="12.75" x14ac:dyDescent="0.15">
       <c r="A12" s="2" t="s">
         <v>15</v>
       </c>
@@ -498,7 +532,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="13">
+    <row r="13" spans="1:2" ht="12.75" x14ac:dyDescent="0.15">
       <c r="A13" s="2" t="s">
         <v>17</v>
       </c>
@@ -506,7 +540,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="14">
+    <row r="14" spans="1:2" ht="12.75" x14ac:dyDescent="0.15">
       <c r="A14" s="2" t="s">
         <v>18</v>
       </c>
@@ -514,7 +548,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15">
+    <row r="15" spans="1:2" ht="12.75" x14ac:dyDescent="0.15">
       <c r="A15" s="2" t="s">
         <v>19</v>
       </c>
@@ -522,7 +556,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="16">
+    <row r="16" spans="1:2" ht="12.75" x14ac:dyDescent="0.15">
       <c r="A16" s="2" t="s">
         <v>20</v>
       </c>
@@ -530,7 +564,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="17">
+    <row r="17" spans="1:2" ht="12.75" x14ac:dyDescent="0.15">
       <c r="A17" s="2" t="s">
         <v>22</v>
       </c>
@@ -538,7 +572,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="18">
+    <row r="18" spans="1:2" ht="12.75" x14ac:dyDescent="0.15">
       <c r="A18" s="2" t="s">
         <v>17</v>
       </c>
@@ -546,7 +580,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="19">
+    <row r="19" spans="1:2" ht="12.75" x14ac:dyDescent="0.15">
       <c r="A19" s="2" t="s">
         <v>24</v>
       </c>
@@ -554,7 +588,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="20">
+    <row r="20" spans="1:2" ht="12.75" x14ac:dyDescent="0.15">
       <c r="A20" s="2" t="s">
         <v>26</v>
       </c>
@@ -562,7 +596,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="21">
+    <row r="21" spans="1:2" ht="12.75" x14ac:dyDescent="0.15">
       <c r="A21" s="2" t="s">
         <v>27</v>
       </c>
@@ -570,7 +604,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="22">
+    <row r="22" spans="1:2" ht="12.75" x14ac:dyDescent="0.15">
       <c r="A22" s="2" t="s">
         <v>28</v>
       </c>
@@ -578,7 +612,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="23">
+    <row r="23" spans="1:2" ht="12.75" x14ac:dyDescent="0.15">
       <c r="A23" s="2" t="s">
         <v>29</v>
       </c>
@@ -586,7 +620,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="24">
+    <row r="24" spans="1:2" ht="12.75" x14ac:dyDescent="0.15">
       <c r="A24" s="2" t="s">
         <v>30</v>
       </c>
@@ -594,7 +628,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="25">
+    <row r="25" spans="1:2" ht="12.75" x14ac:dyDescent="0.15">
       <c r="A25" s="2" t="s">
         <v>31</v>
       </c>
@@ -602,7 +636,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="26">
+    <row r="26" spans="1:2" ht="12.75" x14ac:dyDescent="0.15">
       <c r="A26" s="2" t="s">
         <v>32</v>
       </c>
@@ -610,7 +644,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="27">
+    <row r="27" spans="1:2" ht="12.75" x14ac:dyDescent="0.15">
       <c r="A27" s="2" t="s">
         <v>33</v>
       </c>
@@ -618,7 +652,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="28">
+    <row r="28" spans="1:2" ht="12.75" x14ac:dyDescent="0.15">
       <c r="A28" s="2" t="s">
         <v>34</v>
       </c>
@@ -626,7 +660,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="29">
+    <row r="29" spans="1:2" ht="12.75" x14ac:dyDescent="0.15">
       <c r="A29" s="2" t="s">
         <v>35</v>
       </c>
@@ -634,7 +668,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="30">
+    <row r="30" spans="1:2" ht="12.75" x14ac:dyDescent="0.15">
       <c r="A30" s="2" t="s">
         <v>36</v>
       </c>
@@ -642,7 +676,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="31">
+    <row r="31" spans="1:2" ht="12.75" x14ac:dyDescent="0.15">
       <c r="A31" s="2" t="s">
         <v>37</v>
       </c>
@@ -650,7 +684,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="32">
+    <row r="32" spans="1:2" ht="12.75" x14ac:dyDescent="0.15">
       <c r="A32" s="2" t="s">
         <v>38</v>
       </c>
@@ -658,7 +692,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="33">
+    <row r="33" spans="1:2" ht="12.75" x14ac:dyDescent="0.15">
       <c r="A33" s="2" t="s">
         <v>39</v>
       </c>
@@ -666,7 +700,15 @@
         <v>40</v>
       </c>
     </row>
+    <row r="34" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A34" t="s">
+        <v>41</v>
+      </c>
+      <c r="B34" t="s">
+        <v>42</v>
+      </c>
+    </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>